<commit_message>
Reduced number of rows in excel
</commit_message>
<xml_diff>
--- a/StockData.xlsx
+++ b/StockData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakas\eclipse-workspace\StockMarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D3E6C4E-9054-4BFA-99B9-C680FD7D46DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7814E23-85B3-49A9-B8B1-C88D17173E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6E690734-FE18-4A91-9B61-091B9C2706A4}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Original Value</t>
   </si>
@@ -48,60 +48,20 @@
     <t>HDFC</t>
   </si>
   <si>
-    <t>GAIL</t>
-  </si>
-  <si>
-    <t>ICICI</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>1250.00</t>
-  </si>
-  <si>
-    <t>125.00</t>
-  </si>
-  <si>
-    <t>510.00</t>
-  </si>
-  <si>
-    <t>1262.65</t>
-  </si>
-  <si>
-    <t>124.70</t>
-  </si>
-  <si>
-    <t>519.10</t>
-  </si>
-  <si>
     <t>1260.00</t>
   </si>
   <si>
     <t>1271.95</t>
-  </si>
-  <si>
-    <t>122.55</t>
-  </si>
-  <si>
-    <t>500.00</t>
-  </si>
-  <si>
-    <t>500.30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,18 +406,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE34BDF5-C747-41DB-A120-C8C087258DC4}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -476,44 +436,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the write method to include it in lopp
</commit_message>
<xml_diff>
--- a/StockData.xlsx
+++ b/StockData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakas\eclipse-workspace\StockMarket\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Original Value</t>
   </si>
@@ -61,7 +61,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,10 +415,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>